<commit_message>
fetch data to excel for unit test
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataSample.xlsx
+++ b/CloudTest/SampleData/DataSample.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\emr-cloud-be(new)\emr-cloud-be\CloudTest\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceCode\SmartKarte_1\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F676AE50-DDAC-47BB-9BF9-D6277DA954C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_INF" sheetId="1" r:id="rId1"/>
+    <sheet name="SANTEI_INF" sheetId="2" r:id="rId2"/>
+    <sheet name="SANTEI_INF_DETAIL" sheetId="3" r:id="rId3"/>
+    <sheet name="ODR_INF" sheetId="5" r:id="rId4"/>
+    <sheet name="ODR_INF_DETAIL" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
   <si>
     <t>HP_ID</t>
   </si>
@@ -132,12 +135,171 @@
   </si>
   <si>
     <t>2020-09-15 00:00:00.000</t>
+  </si>
+  <si>
+    <t>ITEM_CD</t>
+  </si>
+  <si>
+    <t>SEQ_NO</t>
+  </si>
+  <si>
+    <t>ALERT_DAYS</t>
+  </si>
+  <si>
+    <t>ALERT_TERM</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>END_DATE</t>
+  </si>
+  <si>
+    <t>KISAN_SBT</t>
+  </si>
+  <si>
+    <t>KISAN_DATE</t>
+  </si>
+  <si>
+    <t>BYOMEI</t>
+  </si>
+  <si>
+    <t>HOSOKU_COMMENT</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>ItemCdUnitTest</t>
+  </si>
+  <si>
+    <t>ByomeiUnitTest</t>
+  </si>
+  <si>
+    <t>hosokuCommentUnitTest</t>
+  </si>
+  <si>
+    <t>CommentUnitTest</t>
+  </si>
+  <si>
+    <t>RP_NO</t>
+  </si>
+  <si>
+    <t>RP_EDA_NO</t>
+  </si>
+  <si>
+    <t>ROW_NO</t>
+  </si>
+  <si>
+    <t>SIN_KOUI_KBN</t>
+  </si>
+  <si>
+    <t>ITEM_NAME</t>
+  </si>
+  <si>
+    <t>SURYO</t>
+  </si>
+  <si>
+    <t>UNIT_NAME</t>
+  </si>
+  <si>
+    <t>UNIT_SBT</t>
+  </si>
+  <si>
+    <t>TERM_VAL</t>
+  </si>
+  <si>
+    <t>KOHATU_KBN</t>
+  </si>
+  <si>
+    <t>SYOHO_KBN</t>
+  </si>
+  <si>
+    <t>SYOHO_LIMIT_KBN</t>
+  </si>
+  <si>
+    <t>DRUG_KBN</t>
+  </si>
+  <si>
+    <t>YOHO_KBN</t>
+  </si>
+  <si>
+    <t>KOKUJI1</t>
+  </si>
+  <si>
+    <t>KOKUJI2</t>
+  </si>
+  <si>
+    <t>IS_NODSP_RECE</t>
+  </si>
+  <si>
+    <t>IPN_CD</t>
+  </si>
+  <si>
+    <t>IPN_NAME</t>
+  </si>
+  <si>
+    <t>JISSI_KBN</t>
+  </si>
+  <si>
+    <t>JISSI_DATE</t>
+  </si>
+  <si>
+    <t>JISSI_ID</t>
+  </si>
+  <si>
+    <t>JISSI_MACHINE</t>
+  </si>
+  <si>
+    <t>REQ_CD</t>
+  </si>
+  <si>
+    <t>BUNKATU</t>
+  </si>
+  <si>
+    <t>CMT_NAME</t>
+  </si>
+  <si>
+    <t>CMT_OPT</t>
+  </si>
+  <si>
+    <t>FONT_COLOR</t>
+  </si>
+  <si>
+    <t>COMMENT_NEWLINE</t>
+  </si>
+  <si>
+    <t>ItemNameUnitTest</t>
+  </si>
+  <si>
+    <t>ODR_KOUI_KBN</t>
+  </si>
+  <si>
+    <t>RP_NAME</t>
+  </si>
+  <si>
+    <t>INOUT_KBN</t>
+  </si>
+  <si>
+    <t>SIKYU_KBN</t>
+  </si>
+  <si>
+    <t>SYOHO_SBT</t>
+  </si>
+  <si>
+    <t>TOSEKI_KBN</t>
+  </si>
+  <si>
+    <t>DAYS_CNT</t>
+  </si>
+  <si>
+    <t>SORT_NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,8 +330,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,11 +647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A206C908-B73B-4F57-9BEE-2DB1C5F880C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +672,7 @@
     <col min="20" max="20" width="12" customWidth="1"/>
     <col min="21" max="21" width="13.140625" customWidth="1"/>
     <col min="22" max="22" width="12.140625" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="24" max="24" width="27.5703125" customWidth="1"/>
     <col min="26" max="26" width="16.42578125" customWidth="1"/>
     <col min="28" max="28" width="13.140625" customWidth="1"/>
     <col min="32" max="32" width="15.28515625" customWidth="1"/>
@@ -680,8 +844,8 @@
       <c r="W2">
         <v>0</v>
       </c>
-      <c r="X2" t="s">
-        <v>32</v>
+      <c r="X2" s="1">
+        <v>44089</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -696,6 +860,523 @@
         <v>0</v>
       </c>
       <c r="AF2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>883</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>883</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>99999999</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>20090810</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999999</v>
+      </c>
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>883</v>
+      </c>
+      <c r="F2">
+        <v>20101221</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999999</v>
+      </c>
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>883</v>
+      </c>
+      <c r="G2">
+        <v>20050307</v>
+      </c>
+      <c r="H2">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done excel UT test get Hoken
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataSample.xlsx
+++ b/CloudTest/SampleData/DataSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\emr-cloud-be(new)\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B26706-536A-4CD1-886D-0DAE97B55994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AA4F40-C725-4246-8EDF-0D2A6CFAD978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{1EE0AC96-80AB-44A0-ACE0-FD2CAF1FB7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="RAIIN_INF" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,16 @@
     <sheet name="SIN_RP_INF" sheetId="4" r:id="rId4"/>
     <sheet name="SIN_KOUI_COUNT" sheetId="5" r:id="rId5"/>
     <sheet name="SIN_KOUI_DETAIL" sheetId="6" r:id="rId6"/>
+    <sheet name="HOKEN_MST" sheetId="7" r:id="rId7"/>
+    <sheet name="PT_HOKEN_INF" sheetId="8" r:id="rId8"/>
+    <sheet name="PT_KOHI" sheetId="9" r:id="rId9"/>
+    <sheet name="PT_HOKEN_CHECK" sheetId="10" r:id="rId10"/>
+    <sheet name="PT_INF" sheetId="11" r:id="rId11"/>
+    <sheet name="USER_MST" sheetId="12" r:id="rId12"/>
+    <sheet name="HOKENSYA_MST" sheetId="13" r:id="rId13"/>
+    <sheet name="ROUDOU_MST" sheetId="17" r:id="rId14"/>
+    <sheet name="PT_ROUSAI_TENKI" sheetId="14" r:id="rId15"/>
+    <sheet name="PT_HOKEN_PATTERN" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="464">
   <si>
     <t>HP_ID</t>
   </si>
@@ -845,12 +855,600 @@
   </si>
   <si>
     <t>再診（診療所）</t>
+  </si>
+  <si>
+    <t>PREF_NO</t>
+  </si>
+  <si>
+    <t>HOKEN_NO</t>
+  </si>
+  <si>
+    <t>HOKEN_EDA_NO</t>
+  </si>
+  <si>
+    <t>SORT_NO</t>
+  </si>
+  <si>
+    <t>HOKEN_SBT_KBN</t>
+  </si>
+  <si>
+    <t>HOUBETU</t>
+  </si>
+  <si>
+    <t>HOKEN_NAME</t>
+  </si>
+  <si>
+    <t>HOKEN_SNAME</t>
+  </si>
+  <si>
+    <t>HOKEN_NAME_CD</t>
+  </si>
+  <si>
+    <t>CHECK_DIGIT</t>
+  </si>
+  <si>
+    <t>JYUKYU_CHECK_DIGIT</t>
+  </si>
+  <si>
+    <t>IS_FUTANSYA_NO_CHECK</t>
+  </si>
+  <si>
+    <t>IS_JYUKYUSYA_NO_CHECK</t>
+  </si>
+  <si>
+    <t>IS_TOKUSYU_NO_CHECK</t>
+  </si>
+  <si>
+    <t>IS_LIMIT_LIST</t>
+  </si>
+  <si>
+    <t>IS_LIMIT_LIST_SUM</t>
+  </si>
+  <si>
+    <t>IS_OTHER_PREF_VALID</t>
+  </si>
+  <si>
+    <t>AGE_START</t>
+  </si>
+  <si>
+    <t>AGE_END</t>
+  </si>
+  <si>
+    <t>EN_TEN</t>
+  </si>
+  <si>
+    <t>SEIKYU_YM</t>
+  </si>
+  <si>
+    <t>RECE_SP_KBN</t>
+  </si>
+  <si>
+    <t>RECE_SEIKYU_KBN</t>
+  </si>
+  <si>
+    <t>RECE_FUTAN_ROUND</t>
+  </si>
+  <si>
+    <t>RECE_KISAI</t>
+  </si>
+  <si>
+    <t>RECE_ZERO_KISAI</t>
+  </si>
+  <si>
+    <t>RECE_FUTAN_KBN</t>
+  </si>
+  <si>
+    <t>RECE_TEN_KISAI</t>
+  </si>
+  <si>
+    <t>CALC_SP_KBN</t>
+  </si>
+  <si>
+    <t>LIMIT_KBN</t>
+  </si>
+  <si>
+    <t>COUNT_KBN</t>
+  </si>
+  <si>
+    <t>FUTAN_KBN</t>
+  </si>
+  <si>
+    <t>FUTAN_RATE</t>
+  </si>
+  <si>
+    <t>KAI_FUTANGAKU</t>
+  </si>
+  <si>
+    <t>KAI_LIMIT_FUTAN</t>
+  </si>
+  <si>
+    <t>DAY_LIMIT_FUTAN</t>
+  </si>
+  <si>
+    <t>DAY_LIMIT_COUNT</t>
+  </si>
+  <si>
+    <t>MONTH_LIMIT_FUTAN</t>
+  </si>
+  <si>
+    <t>MONTH_LIMIT_COUNT</t>
+  </si>
+  <si>
+    <t>KOGAKU_TEKIYO</t>
+  </si>
+  <si>
+    <t>HOKEN_KOHI_KBN</t>
+  </si>
+  <si>
+    <t>MONTH_SP_LIMIT</t>
+  </si>
+  <si>
+    <t>RECE_KISAI2</t>
+  </si>
+  <si>
+    <t>RECE_FUTAN_HIDE</t>
+  </si>
+  <si>
+    <t>KOGAKU_TOTAL_KBN</t>
+  </si>
+  <si>
+    <t>FUTAN_YUSEN</t>
+  </si>
+  <si>
+    <t>KOGAKU_TOTAL_ALL</t>
+  </si>
+  <si>
+    <t>RECE_KISAI_KOKHO</t>
+  </si>
+  <si>
+    <t>KOGAKU_HAIRYO_KBN</t>
+  </si>
+  <si>
+    <t>KOGAKU_TOTAL_EXC_FUTAN</t>
+  </si>
+  <si>
+    <t>2021-12-20 00:00:00.000</t>
+  </si>
+  <si>
+    <t>こども医療費</t>
+  </si>
+  <si>
+    <t>こども(初診1000)</t>
+  </si>
+  <si>
+    <t>こども</t>
+  </si>
+  <si>
+    <t>HOKEN_ID</t>
+  </si>
+  <si>
+    <t>HOKENSYA_NO</t>
+  </si>
+  <si>
+    <t>KIGO</t>
+  </si>
+  <si>
+    <t>BANGO</t>
+  </si>
+  <si>
+    <t>HONKE_KBN</t>
+  </si>
+  <si>
+    <t>HOKENSYA_NAME</t>
+  </si>
+  <si>
+    <t>HOKENSYA_POST</t>
+  </si>
+  <si>
+    <t>HOKENSYA_ADDRESS</t>
+  </si>
+  <si>
+    <t>HOKENSYA_TEL</t>
+  </si>
+  <si>
+    <t>KEIZOKU_KBN</t>
+  </si>
+  <si>
+    <t>SIKAKU_DATE</t>
+  </si>
+  <si>
+    <t>KOFU_DATE</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>GENDOGAKU</t>
+  </si>
+  <si>
+    <t>KOGAKU_KBN</t>
+  </si>
+  <si>
+    <t>KOGAKU_TYPE</t>
+  </si>
+  <si>
+    <t>TOKUREI_YM1</t>
+  </si>
+  <si>
+    <t>TOKUREI_YM2</t>
+  </si>
+  <si>
+    <t>TASUKAI_YM</t>
+  </si>
+  <si>
+    <t>SYOKUMU_KBN</t>
+  </si>
+  <si>
+    <t>GENMEN_KBN</t>
+  </si>
+  <si>
+    <t>GENMEN_RATE</t>
+  </si>
+  <si>
+    <t>GENMEN_GAKU</t>
+  </si>
+  <si>
+    <t>TOKKI1</t>
+  </si>
+  <si>
+    <t>TOKKI2</t>
+  </si>
+  <si>
+    <t>TOKKI3</t>
+  </si>
+  <si>
+    <t>TOKKI4</t>
+  </si>
+  <si>
+    <t>TOKKI5</t>
+  </si>
+  <si>
+    <t>ROUSAI_KOFU_NO</t>
+  </si>
+  <si>
+    <t>ROUSAI_SAIGAI_KBN</t>
+  </si>
+  <si>
+    <t>ROUSAI_JIGYOSYO_NAME</t>
+  </si>
+  <si>
+    <t>ROUSAI_PREF_NAME</t>
+  </si>
+  <si>
+    <t>ROUSAI_CITY_NAME</t>
+  </si>
+  <si>
+    <t>ROUSAI_SYOBYO_DATE</t>
+  </si>
+  <si>
+    <t>ROUSAI_SYOBYO_CD</t>
+  </si>
+  <si>
+    <t>ROUSAI_ROUDOU_CD</t>
+  </si>
+  <si>
+    <t>ROUSAI_KANTOKU_CD</t>
+  </si>
+  <si>
+    <t>ROUSAI_RECE_COUNT</t>
+  </si>
+  <si>
+    <t>JIBAI_HOKEN_NAME</t>
+  </si>
+  <si>
+    <t>JIBAI_HOKEN_TANTO</t>
+  </si>
+  <si>
+    <t>JIBAI_HOKEN_TEL</t>
+  </si>
+  <si>
+    <t>JIBAI_JYUSYOU_DATE</t>
+  </si>
+  <si>
+    <t>RYOYO_START_DATE</t>
+  </si>
+  <si>
+    <t>RYOYO_END_DATE</t>
+  </si>
+  <si>
+    <t>EDA_NO</t>
+  </si>
+  <si>
+    <t>2003-12-11 20:58:07.000</t>
+  </si>
+  <si>
+    <t>2021-02-26 16:20:13.000</t>
+  </si>
+  <si>
+    <t>FUTANSYA_NO</t>
+  </si>
+  <si>
+    <t>JYUKYUSYA_NO</t>
+  </si>
+  <si>
+    <t>TOKUSYU_NO</t>
+  </si>
+  <si>
+    <t>2019-05-07 17:13:08.000</t>
+  </si>
+  <si>
+    <t>2019-10-02 17:32:07.000</t>
+  </si>
+  <si>
+    <t>HOKEN_GRP</t>
+  </si>
+  <si>
+    <t>CHECK_DATE</t>
+  </si>
+  <si>
+    <t>CHECK_ID</t>
+  </si>
+  <si>
+    <t>CHECK_MACHINE</t>
+  </si>
+  <si>
+    <t>CHECK_CMT</t>
+  </si>
+  <si>
+    <t>PT_NUM</t>
+  </si>
+  <si>
+    <t>KANA_NAME</t>
+  </si>
+  <si>
+    <t>SEX</t>
+  </si>
+  <si>
+    <t>BIRTHDAY</t>
+  </si>
+  <si>
+    <t>IS_DEAD</t>
+  </si>
+  <si>
+    <t>DEATH_DATE</t>
+  </si>
+  <si>
+    <t>HOME_POST</t>
+  </si>
+  <si>
+    <t>HOME_ADDRESS1</t>
+  </si>
+  <si>
+    <t>HOME_ADDRESS2</t>
+  </si>
+  <si>
+    <t>TEL1</t>
+  </si>
+  <si>
+    <t>TEL2</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>SETAINUSI</t>
+  </si>
+  <si>
+    <t>ZOKUGARA</t>
+  </si>
+  <si>
+    <t>JOB</t>
+  </si>
+  <si>
+    <t>RENRAKU_NAME</t>
+  </si>
+  <si>
+    <t>RENRAKU_POST</t>
+  </si>
+  <si>
+    <t>RENRAKU_ADDRESS1</t>
+  </si>
+  <si>
+    <t>RENRAKU_ADDRESS2</t>
+  </si>
+  <si>
+    <t>RENRAKU_TEL</t>
+  </si>
+  <si>
+    <t>RENRAKU_MEMO</t>
+  </si>
+  <si>
+    <t>OFFICE_NAME</t>
+  </si>
+  <si>
+    <t>OFFICE_POST</t>
+  </si>
+  <si>
+    <t>OFFICE_ADDRESS1</t>
+  </si>
+  <si>
+    <t>OFFICE_ADDRESS2</t>
+  </si>
+  <si>
+    <t>OFFICE_TEL</t>
+  </si>
+  <si>
+    <t>OFFICE_MEMO</t>
+  </si>
+  <si>
+    <t>IS_RYOSYO_DETAIL</t>
+  </si>
+  <si>
+    <t>PRIMARY_DOCTOR</t>
+  </si>
+  <si>
+    <t>IS_TESTER</t>
+  </si>
+  <si>
+    <t>IS_DELETE</t>
+  </si>
+  <si>
+    <t>MAIN_HOKEN_PID</t>
+  </si>
+  <si>
+    <t>REFERENCE_NO</t>
+  </si>
+  <si>
+    <t>LIMIT_CONS_FLG</t>
+  </si>
+  <si>
+    <t>070-0123-4567</t>
+  </si>
+  <si>
+    <t>2013-10-16 22:43:58.000</t>
+  </si>
+  <si>
+    <t>2021-08-23 12:07:09.000</t>
+  </si>
+  <si>
+    <t>6163OONS32</t>
+  </si>
+  <si>
+    <t>USER_ID</t>
+  </si>
+  <si>
+    <t>JOB_CD</t>
+  </si>
+  <si>
+    <t>MANAGER_KBN</t>
+  </si>
+  <si>
+    <t>SNAME</t>
+  </si>
+  <si>
+    <t>LOGIN_ID</t>
+  </si>
+  <si>
+    <t>LOGIN_PASS</t>
+  </si>
+  <si>
+    <t>MAYAKU_LICENSE_NO</t>
+  </si>
+  <si>
+    <t>DR_NAME</t>
+  </si>
+  <si>
+    <t>2022-05-23 11:29:46.411</t>
+  </si>
+  <si>
+    <t>6163OONS80</t>
+  </si>
+  <si>
+    <t>2022-05-23 11:29:46.412</t>
+  </si>
+  <si>
+    <t>HOUBETU_KBN</t>
+  </si>
+  <si>
+    <t>RATE_HONNIN</t>
+  </si>
+  <si>
+    <t>RATE_KAZOKU</t>
+  </si>
+  <si>
+    <t>POST_CODE</t>
+  </si>
+  <si>
+    <t>ADDRESS1</t>
+  </si>
+  <si>
+    <t>ADDRESS2</t>
+  </si>
+  <si>
+    <t>DELETE_DATE</t>
+  </si>
+  <si>
+    <t>IS_KIGO_NA</t>
+  </si>
+  <si>
+    <t>03-5212-8211</t>
+  </si>
+  <si>
+    <t>2013-06-06 00:00:00.000</t>
+  </si>
+  <si>
+    <t>SINKEI</t>
+  </si>
+  <si>
+    <t>TENKI</t>
+  </si>
+  <si>
+    <t>2022-10-24 09:26:23.530</t>
+  </si>
+  <si>
+    <t>ComputerName</t>
+  </si>
+  <si>
+    <t>HOKEN_SBT_CD</t>
+  </si>
+  <si>
+    <t>KOHI1_ID</t>
+  </si>
+  <si>
+    <t>KOHI2_ID</t>
+  </si>
+  <si>
+    <t>KOHI3_ID</t>
+  </si>
+  <si>
+    <t>KOHI4_ID</t>
+  </si>
+  <si>
+    <t>HOKEN_MEMO</t>
+  </si>
+  <si>
+    <t>2013-10-21 12:10:42.000</t>
+  </si>
+  <si>
+    <t>2021-05-13 11:06:30.000</t>
+  </si>
+  <si>
+    <t>ｶﾝｼﾞｬ 397</t>
+  </si>
+  <si>
+    <t>ﾔﾌﾞ ﾄﾓｺ</t>
+  </si>
+  <si>
+    <t>2022-12-15 07:00:00.000</t>
+  </si>
+  <si>
+    <t>2022-12-16 10:36:28.940</t>
+  </si>
+  <si>
+    <t>全国健康保険協会</t>
+  </si>
+  <si>
+    <t>ｾﾞﾝｺｸｹﾝｺｳﾎｹﾝｷｮｳｶｲ</t>
+  </si>
+  <si>
+    <t>千代田区九段北４－２－１</t>
+  </si>
+  <si>
+    <t>市ヶ谷東急ビル</t>
+  </si>
+  <si>
+    <t>ROUDOU_CD</t>
+  </si>
+  <si>
+    <t>ROUDOU_NAME</t>
+  </si>
+  <si>
+    <t>2016-10-14 00:00:00.000</t>
+  </si>
+  <si>
+    <t>北海道</t>
+  </si>
+  <si>
+    <t>01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -881,9 +1479,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,6 +2017,957 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AAFF5E-1553-423A-8948-5BABD26D3D84}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I1" t="s">
+        <v>379</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>99999</v>
+      </c>
+      <c r="E2">
+        <v>594453</v>
+      </c>
+      <c r="F2" t="s">
+        <v>453</v>
+      </c>
+      <c r="G2">
+        <v>99999</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>454</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <f>G2</f>
+        <v>99999</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EA7E5D-5876-4E84-8E29-B9F2D3C3E653}">
+  <dimension ref="A1:AR2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I1" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K1" t="s">
+        <v>386</v>
+      </c>
+      <c r="L1" t="s">
+        <v>387</v>
+      </c>
+      <c r="M1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N1" t="s">
+        <v>389</v>
+      </c>
+      <c r="O1" t="s">
+        <v>390</v>
+      </c>
+      <c r="P1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>392</v>
+      </c>
+      <c r="R1" t="s">
+        <v>393</v>
+      </c>
+      <c r="S1" t="s">
+        <v>394</v>
+      </c>
+      <c r="T1" t="s">
+        <v>395</v>
+      </c>
+      <c r="U1" t="s">
+        <v>396</v>
+      </c>
+      <c r="V1" t="s">
+        <v>397</v>
+      </c>
+      <c r="W1" t="s">
+        <v>398</v>
+      </c>
+      <c r="X1" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>402</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>403</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>404</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>405</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>406</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>407</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>408</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>409</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>410</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>411</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>932</v>
+      </c>
+      <c r="D2">
+        <v>397</v>
+      </c>
+      <c r="E2" t="s">
+        <v>451</v>
+      </c>
+      <c r="F2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>19420308</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>415</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AN2">
+        <v>186</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2892F96D-4BBB-4A2B-89D1-DCE074D5AF81}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>421</v>
+      </c>
+      <c r="J1" t="s">
+        <v>422</v>
+      </c>
+      <c r="K1" t="s">
+        <v>423</v>
+      </c>
+      <c r="L1" t="s">
+        <v>424</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>272</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
+        <v>201</v>
+      </c>
+      <c r="X1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>295</v>
+      </c>
+      <c r="C2">
+        <v>99999</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>452</v>
+      </c>
+      <c r="H2" t="s">
+        <v>452</v>
+      </c>
+      <c r="I2" t="s">
+        <v>452</v>
+      </c>
+      <c r="J2">
+        <v>287</v>
+      </c>
+      <c r="K2">
+        <v>287</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>99999999</v>
+      </c>
+      <c r="O2">
+        <v>286</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>426</v>
+      </c>
+      <c r="R2">
+        <v>186</v>
+      </c>
+      <c r="S2" t="s">
+        <v>427</v>
+      </c>
+      <c r="T2" t="s">
+        <v>428</v>
+      </c>
+      <c r="U2">
+        <v>186</v>
+      </c>
+      <c r="V2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39969BAD-2255-4590-A481-753CD7492ECB}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" t="s">
+        <v>326</v>
+      </c>
+      <c r="K1" t="s">
+        <v>430</v>
+      </c>
+      <c r="L1" t="s">
+        <v>431</v>
+      </c>
+      <c r="M1" t="s">
+        <v>432</v>
+      </c>
+      <c r="N1" t="s">
+        <v>433</v>
+      </c>
+      <c r="O1" t="s">
+        <v>434</v>
+      </c>
+      <c r="P1" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>435</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1000009</v>
+      </c>
+      <c r="C2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" t="s">
+        <v>456</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1028575</v>
+      </c>
+      <c r="N2" t="s">
+        <v>457</v>
+      </c>
+      <c r="O2" t="s">
+        <v>458</v>
+      </c>
+      <c r="P2" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>438</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>438</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC06F9-B56A-49DC-8DA6-70D5C7DCEB9C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80339B3E-C46C-4F5F-965E-FBFD75439185}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>99999</v>
+      </c>
+      <c r="D2">
+        <v>10171</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>441</v>
+      </c>
+      <c r="J2">
+        <v>99909</v>
+      </c>
+      <c r="L2" t="s">
+        <v>441</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E6173B-2B54-4FD6-BDDC-E47DE7F4F556}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I1" t="s">
+        <v>445</v>
+      </c>
+      <c r="J1" t="s">
+        <v>446</v>
+      </c>
+      <c r="K1" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>99999</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>99999</v>
+      </c>
+      <c r="H2">
+        <v>888888</v>
+      </c>
+      <c r="I2">
+        <v>666666</v>
+      </c>
+      <c r="J2">
+        <v>333333</v>
+      </c>
+      <c r="K2">
+        <v>777777</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>99999999</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>450</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4904BF98-9085-4855-9DF7-31BF552F8ACF}">
   <dimension ref="A1:U2"/>
@@ -3623,8 +5173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A7406A-BC0C-494B-AAF4-B33C0F46F337}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,7 +5185,7 @@
     <col min="10" max="10" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -3702,7 +5252,7 @@
         <v>54522111111</v>
       </c>
       <c r="C2">
-        <v>20220401</v>
+        <v>202204</v>
       </c>
       <c r="D2">
         <v>1922</v>
@@ -3729,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q2">
         <v>22</v>
@@ -3748,7 +5298,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3811,7 +5361,7 @@
         <v>54522111111</v>
       </c>
       <c r="C2">
-        <v>20220401</v>
+        <v>202204</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -3841,7 +5391,7 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>20050307</v>
+        <v>20220307</v>
       </c>
     </row>
   </sheetData>
@@ -3853,8 +5403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B309D67-BB97-4939-A394-3B8E99A0D15B}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,7 +5520,7 @@
         <v>54522111111</v>
       </c>
       <c r="C2">
-        <v>20220401</v>
+        <v>202204</v>
       </c>
       <c r="D2">
         <v>1922</v>
@@ -3990,7 +5540,7 @@
       <c r="I2" t="s">
         <v>268</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>229</v>
       </c>
       <c r="K2" t="s">
@@ -4022,6 +5572,1095 @@
       </c>
       <c r="AF2" t="s">
         <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14A4ED8-8CA4-4E5D-B593-9F16E6D3AF8B}">
+  <dimension ref="A1:BG2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" t="s">
+        <v>275</v>
+      </c>
+      <c r="K1" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1" t="s">
+        <v>277</v>
+      </c>
+      <c r="M1" t="s">
+        <v>278</v>
+      </c>
+      <c r="N1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O1" t="s">
+        <v>280</v>
+      </c>
+      <c r="P1" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>282</v>
+      </c>
+      <c r="R1" t="s">
+        <v>283</v>
+      </c>
+      <c r="S1" t="s">
+        <v>284</v>
+      </c>
+      <c r="T1" t="s">
+        <v>285</v>
+      </c>
+      <c r="U1" t="s">
+        <v>286</v>
+      </c>
+      <c r="V1" t="s">
+        <v>287</v>
+      </c>
+      <c r="W1" t="s">
+        <v>288</v>
+      </c>
+      <c r="X1" t="s">
+        <v>289</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>290</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>291</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>292</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>293</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>295</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>296</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>297</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>298</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>299</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>300</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>301</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>311</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>312</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>313</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>314</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>315</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>316</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>317</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2">
+        <v>390</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20220101</v>
+      </c>
+      <c r="F2">
+        <v>99999999</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>90</v>
+      </c>
+      <c r="J2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K2" t="s">
+        <v>321</v>
+      </c>
+      <c r="L2" t="s">
+        <v>322</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>999</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>3</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>1000</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>2</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>319</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>319</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>11</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0689A42-EE24-40E3-9D61-7FAA08A3308D}">
+  <dimension ref="A1:BI2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="18" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I1" t="s">
+        <v>326</v>
+      </c>
+      <c r="J1" t="s">
+        <v>327</v>
+      </c>
+      <c r="K1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" t="s">
+        <v>328</v>
+      </c>
+      <c r="N1" t="s">
+        <v>329</v>
+      </c>
+      <c r="O1" t="s">
+        <v>330</v>
+      </c>
+      <c r="P1" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R1" t="s">
+        <v>333</v>
+      </c>
+      <c r="S1" t="s">
+        <v>334</v>
+      </c>
+      <c r="T1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>335</v>
+      </c>
+      <c r="W1" t="s">
+        <v>336</v>
+      </c>
+      <c r="X1" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>348</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>352</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>355</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>356</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>358</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>365</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>366</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>99999</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>390</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1223</v>
+      </c>
+      <c r="H2">
+        <v>123</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>20021212</v>
+      </c>
+      <c r="S2">
+        <v>20021212</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>20130930</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>368</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>369</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D721056-BF6E-4B9A-B45A-56D46289D5AF}">
+  <dimension ref="A1:Y5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" t="s">
+        <v>371</v>
+      </c>
+      <c r="J1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K1" t="s">
+        <v>333</v>
+      </c>
+      <c r="L1" t="s">
+        <v>334</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>335</v>
+      </c>
+      <c r="P1" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+      <c r="C2">
+        <v>888888</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>158</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>58280314</v>
+      </c>
+      <c r="I2">
+        <v>1500255</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>20180701</v>
+      </c>
+      <c r="N2">
+        <v>20190714</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>600</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>373</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>374</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>7</v>
+      </c>
+      <c r="Y2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>999999</v>
+      </c>
+      <c r="C3">
+        <v>666666</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>158</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>58280314</v>
+      </c>
+      <c r="I3">
+        <v>1500255</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>20180701</v>
+      </c>
+      <c r="N3">
+        <v>20190714</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>600</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>373</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>374</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>7</v>
+      </c>
+      <c r="Y3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>999999</v>
+      </c>
+      <c r="C4">
+        <v>333333</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>158</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>58280314</v>
+      </c>
+      <c r="I4">
+        <v>1500255</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>20180701</v>
+      </c>
+      <c r="N4">
+        <v>20190714</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>600</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>373</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>374</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>7</v>
+      </c>
+      <c r="Y4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>999999</v>
+      </c>
+      <c r="C5">
+        <v>777777</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>158</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>58280314</v>
+      </c>
+      <c r="I5">
+        <v>1500255</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>20180701</v>
+      </c>
+      <c r="N5">
+        <v>20190714</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>600</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>373</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>374</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>7</v>
+      </c>
+      <c r="Y5">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update read data from excel for unit test
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/DataSample.xlsx
+++ b/CloudTest/SampleData/DataSample.xlsx
@@ -944,7 +944,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
         <v>47</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1185,7 +1185,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L1" sqref="L1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,7 +1338,7 @@
         <v>77</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M2">
         <v>0</v>

</xml_diff>